<commit_message>
Fix translations formatting parameters
</commit_message>
<xml_diff>
--- a/app/translations.xlsx
+++ b/app/translations.xlsx
@@ -12646,31 +12646,31 @@
     <t>archived_selected_notes_PLURALS_one</t>
   </si>
   <si>
-    <t>Archived %d note</t>
-  </si>
-  <si>
-    <t>%d note archivée</t>
-  </si>
-  <si>
-    <t>Archiviata %d nota</t>
-  </si>
-  <si>
-    <t>Gearchiveerde %d notitie</t>
+    <t>Archived %1$d note</t>
+  </si>
+  <si>
+    <t>%1$d note archivée</t>
+  </si>
+  <si>
+    <t>Archiviata %1$d nota</t>
+  </si>
+  <si>
+    <t>Gearchiveerde %1$d notitie</t>
   </si>
   <si>
     <t>archived_selected_notes_PLURALS_other</t>
   </si>
   <si>
-    <t>Archived %d notes</t>
-  </si>
-  <si>
-    <t>%d notes archivées</t>
-  </si>
-  <si>
-    <t>Archiviate %d note</t>
-  </si>
-  <si>
-    <t>Gearchiveerde %d notities</t>
+    <t>Archived %1$d notes</t>
+  </si>
+  <si>
+    <t>%1$d notes archivées</t>
+  </si>
+  <si>
+    <t>Archiviate %1$d note</t>
+  </si>
+  <si>
+    <t>Gearchiveerde %1$d notities</t>
   </si>
   <si>
     <t>archived_selected_notes_PLURALS_two</t>
@@ -13255,28 +13255,28 @@
     <t>cant_add_files_PLURALS_one</t>
   </si>
   <si>
-    <t>Can’t add %d file</t>
-  </si>
-  <si>
-    <t>%d fichier n\'a pas pu être ajouté</t>
-  </si>
-  <si>
-    <t>Impossibile aggiungere %d file</t>
-  </si>
-  <si>
-    <t>Kan %d bestand niet toevoegen</t>
+    <t>Can’t add %1$d file</t>
+  </si>
+  <si>
+    <t>%1$d fichier n\'a pas pu être ajouté</t>
+  </si>
+  <si>
+    <t>Impossibile aggiungere %1$d file</t>
+  </si>
+  <si>
+    <t>Kan %1$d bestand niet toevoegen</t>
   </si>
   <si>
     <t>cant_add_files_PLURALS_other</t>
   </si>
   <si>
-    <t>Can’t add %d files</t>
-  </si>
-  <si>
-    <t>%d fichiers n\'ont pas pu être ajoutés</t>
-  </si>
-  <si>
-    <t>Kan %d bestanden niet toevoegen</t>
+    <t>Can’t add %1$d files</t>
+  </si>
+  <si>
+    <t>%1$d fichiers n\'ont pas pu être ajoutés</t>
+  </si>
+  <si>
+    <t>Kan %1$d bestanden niet toevoegen</t>
   </si>
   <si>
     <t>cant_add_files_PLURALS_two</t>
@@ -13288,85 +13288,85 @@
     <t>cant_add_images_PLURALS_few</t>
   </si>
   <si>
-    <t>Nepodařilo se přidat %d obrázky</t>
-  </si>
-  <si>
-    <t>Nie można dodać %d obrazów</t>
-  </si>
-  <si>
-    <t>%d slike niso bile dodane.</t>
+    <t>Nepodařilo se přidat %1$d obrázky</t>
+  </si>
+  <si>
+    <t>Nie można dodać %1$d obrazów</t>
+  </si>
+  <si>
+    <t>%1$d slike niso bile dodane.</t>
   </si>
   <si>
     <t>cant_add_images_PLURALS_many</t>
   </si>
   <si>
-    <t>Nepodařilo se přidat %d obrázků</t>
+    <t>Nepodařilo se přidat %1$d obrázků</t>
   </si>
   <si>
     <t>cant_add_images_PLURALS_one</t>
   </si>
   <si>
-    <t>Can’t add %d image</t>
-  </si>
-  <si>
-    <t>Nepodařilo se přidat %d obrázek</t>
-  </si>
-  <si>
-    <t>Kann %d Bild nicht hinzufügen</t>
-  </si>
-  <si>
-    <t>Impossible d\'ajouter %d image</t>
-  </si>
-  <si>
-    <t>Impossibile aggiungere %d immagine</t>
-  </si>
-  <si>
-    <t>Kan ikke legge til %d bilde</t>
-  </si>
-  <si>
-    <t>Kan %d afbeelding niet toevoegen</t>
-  </si>
-  <si>
-    <t>Kan ikkje legga til %d bilete</t>
-  </si>
-  <si>
-    <t>Nie można dodać %d obrazu</t>
-  </si>
-  <si>
-    <t>%d slika ni bila dodana.</t>
-  </si>
-  <si>
-    <t>Không thể thêm %d ảnh</t>
+    <t>Can’t add %1$d image</t>
+  </si>
+  <si>
+    <t>Nepodařilo se přidat %1$d obrázek</t>
+  </si>
+  <si>
+    <t>Kann %1$d Bild nicht hinzufügen</t>
+  </si>
+  <si>
+    <t>Impossible d\'ajouter %1$d image</t>
+  </si>
+  <si>
+    <t>Impossibile aggiungere %1$d immagine</t>
+  </si>
+  <si>
+    <t>Kan ikke legge til %1$d bilde</t>
+  </si>
+  <si>
+    <t>Kan %1$d afbeelding niet toevoegen</t>
+  </si>
+  <si>
+    <t>Kan ikkje legga til %1$d bilete</t>
+  </si>
+  <si>
+    <t>Nie można dodać %1$d obrazu</t>
+  </si>
+  <si>
+    <t>%1$d slika ni bila dodana.</t>
+  </si>
+  <si>
+    <t>Không thể thêm %1$d ảnh</t>
   </si>
   <si>
     <t>cant_add_images_PLURALS_other</t>
   </si>
   <si>
-    <t>Can’t add %d images</t>
-  </si>
-  <si>
-    <t>Kann %d Bilder nicht hinzufügen</t>
-  </si>
-  <si>
-    <t>Impossible d\'ajouter %d images</t>
-  </si>
-  <si>
-    <t>Impossibile aggiungere %d immagini</t>
-  </si>
-  <si>
-    <t>Kan ikke legge til %d bilder</t>
-  </si>
-  <si>
-    <t>Kan %d afbeeldingen niet toevoegen</t>
-  </si>
-  <si>
-    <t>%d slik ni bilo dodanih.</t>
+    <t>Can’t add %1$d images</t>
+  </si>
+  <si>
+    <t>Kann %1$d Bilder nicht hinzufügen</t>
+  </si>
+  <si>
+    <t>Impossible d\'ajouter %1$d images</t>
+  </si>
+  <si>
+    <t>Impossibile aggiungere %1$d immagini</t>
+  </si>
+  <si>
+    <t>Kan ikke legge til %1$d bilder</t>
+  </si>
+  <si>
+    <t>Kan %1$d afbeeldingen niet toevoegen</t>
+  </si>
+  <si>
+    <t>%1$d slik ni bilo dodanih.</t>
   </si>
   <si>
     <t>cant_add_images_PLURALS_two</t>
   </si>
   <si>
-    <t>%d sliki nista bili dodani.</t>
+    <t>%1$d sliki nista bili dodani.</t>
   </si>
   <si>
     <t>cant_add_images_PLURALS_zero</t>
@@ -14803,19 +14803,19 @@
     <t>delete_file</t>
   </si>
   <si>
-    <t>Delete file \'%s\'?</t>
-  </si>
-  <si>
-    <t>Datei \'%s\' löschen?</t>
-  </si>
-  <si>
-    <t>Supprimer le fichier \'%s\'?</t>
-  </si>
-  <si>
-    <t>Eliminare il file \’%s\’?</t>
-  </si>
-  <si>
-    <t>Bestand \'%s\' verwijderen?</t>
+    <t>Delete file \'%1$s\'?</t>
+  </si>
+  <si>
+    <t>Datei \'%1$s\' löschen?</t>
+  </si>
+  <si>
+    <t>Supprimer le fichier \'%1$s\'?</t>
+  </si>
+  <si>
+    <t>Eliminare il file \’%1$s\’?</t>
+  </si>
+  <si>
+    <t>Bestand \'%1$s\' verwijderen?</t>
   </si>
   <si>
     <t>delete_forever</t>
@@ -15250,31 +15250,31 @@
     <t>deleted_selected_notes_PLURALS_one</t>
   </si>
   <si>
-    <t>Deleted %d note</t>
-  </si>
-  <si>
-    <t>%d note supprimée</t>
-  </si>
-  <si>
-    <t>Eliminata %d nota</t>
-  </si>
-  <si>
-    <t>Verwijderde %d notitie</t>
+    <t>Deleted %1$d note</t>
+  </si>
+  <si>
+    <t>%1$d note supprimée</t>
+  </si>
+  <si>
+    <t>Eliminata %1$d nota</t>
+  </si>
+  <si>
+    <t>Verwijderde %1$d notitie</t>
   </si>
   <si>
     <t>deleted_selected_notes_PLURALS_other</t>
   </si>
   <si>
-    <t>Deleted %d notes</t>
-  </si>
-  <si>
-    <t>%d notes supprimées</t>
-  </si>
-  <si>
-    <t>Eliminate %d note</t>
-  </si>
-  <si>
-    <t>Verwijderde %d notities</t>
+    <t>Deleted %1$d notes</t>
+  </si>
+  <si>
+    <t>%1$d notes supprimées</t>
+  </si>
+  <si>
+    <t>Eliminate %1$d note</t>
+  </si>
+  <si>
+    <t>Verwijderde %1$d notities</t>
   </si>
   <si>
     <t>deleted_selected_notes_PLURALS_two</t>
@@ -16874,31 +16874,31 @@
     <t>imported_notes_PLURALS_one</t>
   </si>
   <si>
-    <t>Imported %s Note</t>
-  </si>
-  <si>
-    <t>%s note importée</t>
-  </si>
-  <si>
-    <t>Importata %s nota</t>
-  </si>
-  <si>
-    <t>Geïmporteerde %s Notitie</t>
+    <t>Imported %1$s Note</t>
+  </si>
+  <si>
+    <t>%1$s note importée</t>
+  </si>
+  <si>
+    <t>Importata %1$s nota</t>
+  </si>
+  <si>
+    <t>Geïmporteerde %1$s Notitie</t>
   </si>
   <si>
     <t>imported_notes_PLURALS_other</t>
   </si>
   <si>
-    <t>Imported %s Notes</t>
-  </si>
-  <si>
-    <t>%s notes importées</t>
-  </si>
-  <si>
-    <t>Importate %s note</t>
-  </si>
-  <si>
-    <t>Geïmporteerde %s Notities</t>
+    <t>Imported %1$s Notes</t>
+  </si>
+  <si>
+    <t>%1$s notes importées</t>
+  </si>
+  <si>
+    <t>Importate %1$s note</t>
+  </si>
+  <si>
+    <t>Geïmporteerde %1$s Notities</t>
   </si>
   <si>
     <t>imported_notes_PLURALS_two</t>
@@ -18428,19 +18428,19 @@
     <t>more</t>
   </si>
   <si>
-    <t>%d more</t>
-  </si>
-  <si>
-    <t>%d mehr</t>
-  </si>
-  <si>
-    <t>%d de plus</t>
-  </si>
-  <si>
-    <t>…ancora %d</t>
-  </si>
-  <si>
-    <t>%d meer</t>
+    <t>%1$d more</t>
+  </si>
+  <si>
+    <t>%1$d mehr</t>
+  </si>
+  <si>
+    <t>%1$d de plus</t>
+  </si>
+  <si>
+    <t>…ancora %1$d</t>
+  </si>
+  <si>
+    <t>%1$d meer</t>
   </si>
   <si>
     <t>more_files_PLURALS_few</t>
@@ -18452,37 +18452,37 @@
     <t>more_files_PLURALS_one</t>
   </si>
   <si>
-    <t>…%d more file</t>
-  </si>
-  <si>
-    <t>…%d weitere Datei</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…et %d fichier </t>
-  </si>
-  <si>
-    <t>…%d altro file</t>
-  </si>
-  <si>
-    <t>…%d ander bestand</t>
+    <t>…%1$d more file</t>
+  </si>
+  <si>
+    <t>…%1$d weitere Datei</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…et %1$d fichier </t>
+  </si>
+  <si>
+    <t>…%1$d altro file</t>
+  </si>
+  <si>
+    <t>…%1$d ander bestand</t>
   </si>
   <si>
     <t>more_files_PLURALS_other</t>
   </si>
   <si>
-    <t>…%d more files</t>
-  </si>
-  <si>
-    <t>…%d weitere Dateien</t>
-  </si>
-  <si>
-    <t>…et %d fichiers</t>
-  </si>
-  <si>
-    <t>…altri %d file</t>
-  </si>
-  <si>
-    <t>…%d andere bestanden</t>
+    <t>…%1$d more files</t>
+  </si>
+  <si>
+    <t>…%1$d weitere Dateien</t>
+  </si>
+  <si>
+    <t>…et %1$d fichiers</t>
+  </si>
+  <si>
+    <t>…altri %1$d file</t>
+  </si>
+  <si>
+    <t>…%1$d andere bestanden</t>
   </si>
   <si>
     <t>more_files_PLURALS_two</t>
@@ -19550,31 +19550,31 @@
     <t>restored_selected_notes_PLURALS_one</t>
   </si>
   <si>
-    <t>Restored %d note</t>
-  </si>
-  <si>
-    <t>%d note restaurée</t>
-  </si>
-  <si>
-    <t>Ripristinata %d nota</t>
-  </si>
-  <si>
-    <t>Herstelde %d notitie</t>
+    <t>Restored %1$d note</t>
+  </si>
+  <si>
+    <t>%1$d note restaurée</t>
+  </si>
+  <si>
+    <t>Ripristinata %1$d nota</t>
+  </si>
+  <si>
+    <t>Herstelde %1$d notitie</t>
   </si>
   <si>
     <t>restored_selected_notes_PLURALS_other</t>
   </si>
   <si>
-    <t>Restored %d notes</t>
-  </si>
-  <si>
-    <t>%d notes restaurées</t>
-  </si>
-  <si>
-    <t>Ripristinate %d note</t>
-  </si>
-  <si>
-    <t>Herstelde %d notities</t>
+    <t>Restored %1$d notes</t>
+  </si>
+  <si>
+    <t>%1$d notes restaurées</t>
+  </si>
+  <si>
+    <t>Ripristinate %1$d note</t>
+  </si>
+  <si>
+    <t>Herstelde %1$d notities</t>
   </si>
   <si>
     <t>restored_selected_notes_PLURALS_two</t>
@@ -21125,31 +21125,31 @@
     <t>unarchived_selected_notes_PLURALS_one</t>
   </si>
   <si>
-    <t>Unarchived %d note</t>
-  </si>
-  <si>
-    <t>%d note désarchivée</t>
-  </si>
-  <si>
-    <t>Annullata archiviazione di %d nota</t>
-  </si>
-  <si>
-    <t>De-gearchiveerde %d notitie</t>
+    <t>Unarchived %1$d note</t>
+  </si>
+  <si>
+    <t>%1$d note désarchivée</t>
+  </si>
+  <si>
+    <t>Annullata archiviazione di %1$d nota</t>
+  </si>
+  <si>
+    <t>De-gearchiveerde %1$d notitie</t>
   </si>
   <si>
     <t>unarchived_selected_notes_PLURALS_other</t>
   </si>
   <si>
-    <t>Unarchived %d notes</t>
-  </si>
-  <si>
-    <t>%d notes désarchivées</t>
-  </si>
-  <si>
-    <t>Annullata archiviazione di %d note</t>
-  </si>
-  <si>
-    <t>De-gearchiveerde %d notities</t>
+    <t>Unarchived %1$d notes</t>
+  </si>
+  <si>
+    <t>%1$d notes désarchivées</t>
+  </si>
+  <si>
+    <t>Annullata archiviazione di %1$d note</t>
+  </si>
+  <si>
+    <t>De-gearchiveerde %1$d notities</t>
   </si>
   <si>
     <t>unarchived_selected_notes_PLURALS_two</t>

</xml_diff>

<commit_message>
Remove removed translations from cs/strings.xml
</commit_message>
<xml_diff>
--- a/app/translations.xlsx
+++ b/app/translations.xlsx
@@ -9,7 +9,7 @@
     <sheet name="Translations" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Translations!$A$1:$AF$321</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Translations!$A$1:$AF$317</definedName>
   </definedNames>
 </workbook>
 </file>
@@ -11951,7 +11951,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9951" uniqueCount="3488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9827" uniqueCount="3480">
   <si>
     <t>Key</t>
   </si>
@@ -22392,30 +22392,6 @@
   </si>
   <si>
     <t>不会删除与此标签相关联的笔记</t>
-  </si>
-  <si>
-    <t>data_on_external</t>
-  </si>
-  <si>
-    <t>Ukládat data na externí úložiště</t>
-  </si>
-  <si>
-    <t>disable_auto_backup</t>
-  </si>
-  <si>
-    <t>Zakázat automatickou zálohu</t>
-  </si>
-  <si>
-    <t>disable_external_data</t>
-  </si>
-  <si>
-    <t>Přesunout data zpět na interní uložiště</t>
-  </si>
-  <si>
-    <t>external_data_message</t>
-  </si>
-  <si>
-    <t>Povolením této funkce se interní databáze aplikace přesune do externího úložiště aplikace (Android/media/com.philkes.notallyx).\nV kombinaci s aplikacemi pro synchronizaci souborů lze tuto funkci použít k synchronizaci dat NotallyX mezi více zařízeními.</t>
   </si>
 </sst>
 </file>
@@ -26528,7 +26504,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AE321"/>
+  <dimension ref="A1:AE317"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="3.0" ySplit="1.0" state="frozen" topLeftCell="D2" activePane="bottomRight"/>
@@ -56656,388 +56632,8 @@
         <v>3479</v>
       </c>
     </row>
-    <row r="318">
-      <c r="A318" t="s" s="1">
-        <v>3480</v>
-      </c>
-      <c r="B318" t="s" s="1">
-        <v>32</v>
-      </c>
-      <c r="C318" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="D318" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="E318" t="s" s="1">
-        <v>3481</v>
-      </c>
-      <c r="F318" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="G318" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="H318" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="I318" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="J318" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="K318" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="L318" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="M318" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="N318" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="O318" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="P318" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="Q318" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="R318" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="S318" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="T318" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="U318" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="V318" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="W318" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="X318" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="Y318" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="Z318" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="AA318" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="AB318" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="AC318" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="AD318" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="AE318" t="s" s="2">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="319">
-      <c r="A319" t="s" s="1">
-        <v>3482</v>
-      </c>
-      <c r="B319" t="s" s="1">
-        <v>32</v>
-      </c>
-      <c r="C319" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="D319" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="E319" t="s" s="1">
-        <v>3483</v>
-      </c>
-      <c r="F319" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="G319" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="H319" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="I319" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="J319" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="K319" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="L319" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="M319" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="N319" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="O319" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="P319" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="Q319" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="R319" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="S319" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="T319" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="U319" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="V319" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="W319" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="X319" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="Y319" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="Z319" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="AA319" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="AB319" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="AC319" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="AD319" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="AE319" t="s" s="2">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="320">
-      <c r="A320" t="s" s="1">
-        <v>3484</v>
-      </c>
-      <c r="B320" t="s" s="1">
-        <v>32</v>
-      </c>
-      <c r="C320" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="D320" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="E320" t="s" s="1">
-        <v>3485</v>
-      </c>
-      <c r="F320" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="G320" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="H320" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="I320" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="J320" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="K320" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="L320" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="M320" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="N320" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="O320" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="P320" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="Q320" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="R320" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="S320" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="T320" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="U320" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="V320" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="W320" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="X320" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="Y320" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="Z320" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="AA320" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="AB320" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="AC320" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="AD320" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="AE320" t="s" s="2">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="321">
-      <c r="A321" t="s" s="1">
-        <v>3486</v>
-      </c>
-      <c r="B321" t="s" s="1">
-        <v>32</v>
-      </c>
-      <c r="C321" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="D321" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="E321" t="s" s="1">
-        <v>3487</v>
-      </c>
-      <c r="F321" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="G321" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="H321" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="I321" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="J321" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="K321" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="L321" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="M321" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="N321" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="O321" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="P321" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="Q321" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="R321" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="S321" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="T321" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="U321" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="V321" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="W321" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="X321" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="Y321" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="Z321" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="AA321" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="AB321" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="AC321" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="AD321" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="AE321" t="s" s="2">
-        <v>61</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:AF321"/>
+  <autoFilter ref="A1:AF317"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId3"/>

</xml_diff>

<commit_message>
Fix german auto_backup_error_message translation
</commit_message>
<xml_diff>
--- a/app/translations.xlsx
+++ b/app/translations.xlsx
@@ -12893,7 +12893,9 @@
 Prosím, zkontrolujte nastavení nebo nahlaste chybu</t>
   </si>
   <si>
-    <t>Überprüfe deine Einstellungen oder melde einen Bug</t>
+    <t>Beim autom. Backup ist ein Fehler aufgetreten:
+'%1$s'
+Überprüfe deine Einstellungen oder melde einen Bug</t>
   </si>
   <si>
     <t>Ha ocurrido un error durante una copia automática:

</xml_diff>

<commit_message>
Add option to always show search bar expanded
</commit_message>
<xml_diff>
--- a/app/translations.xlsx
+++ b/app/translations.xlsx
@@ -9,7 +9,7 @@
     <sheet name="Translations" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Translations!$A$1:$AG$345</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Translations!$A$1:$AG$347</definedName>
   </definedNames>
 </workbook>
 </file>
@@ -12335,7 +12335,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11040" uniqueCount="5065">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11104" uniqueCount="5069">
   <si>
     <t>Key</t>
   </si>
@@ -27658,6 +27658,18 @@
   </si>
   <si>
     <t>不會刪除與此標籤相關的筆記</t>
+  </si>
+  <si>
+    <t>always_show_search_bar</t>
+  </si>
+  <si>
+    <t>Always show search bar expanded</t>
+  </si>
+  <si>
+    <t>always_show_search_bar_hint</t>
+  </si>
+  <si>
+    <t>By enabling this, the search bar will always be shown in the layout instead of using a search icon in the top bar</t>
   </si>
 </sst>
 </file>
@@ -31898,7 +31910,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AF345"/>
+  <dimension ref="A1:AF347"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="3.0" ySplit="1.0" state="frozen" topLeftCell="D2" activePane="bottomRight"/>
@@ -65721,8 +65733,204 @@
         <v>5064</v>
       </c>
     </row>
+    <row r="346">
+      <c r="A346" t="s" s="1">
+        <v>5065</v>
+      </c>
+      <c r="B346" t="s" s="1">
+        <v>33</v>
+      </c>
+      <c r="C346" t="s" s="1">
+        <v>5066</v>
+      </c>
+      <c r="D346" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E346" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="F346" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="G346" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="H346" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="I346" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="J346" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="K346" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="L346" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="M346" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="N346" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="O346" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="P346" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="Q346" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="R346" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="S346" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="T346" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="U346" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="V346" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="W346" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="X346" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="Y346" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="Z346" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="AA346" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="AB346" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="AC346" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="AD346" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="AE346" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="AF346" t="s" s="2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="s" s="1">
+        <v>5067</v>
+      </c>
+      <c r="B347" t="s" s="1">
+        <v>33</v>
+      </c>
+      <c r="C347" t="s" s="1">
+        <v>5068</v>
+      </c>
+      <c r="D347" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E347" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="F347" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="G347" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="H347" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="I347" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="J347" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="K347" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="L347" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="M347" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="N347" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="O347" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="P347" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="Q347" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="R347" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="S347" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="T347" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="U347" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="V347" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="W347" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="X347" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="Y347" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="Z347" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="AA347" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="AB347" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="AC347" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="AD347" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="AE347" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="AF347" t="s" s="2">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:AG345"/>
+  <autoFilter ref="A1:AG347"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId3"/>

</xml_diff>

<commit_message>
Add Markdown import and export
</commit_message>
<xml_diff>
--- a/app/translations.xlsx
+++ b/app/translations.xlsx
@@ -25180,43 +25180,43 @@
     <t>plain_text_files</t>
   </si>
   <si>
-    <t>Plain Text Files</t>
-  </si>
-  <si>
-    <t>Textové soubory</t>
-  </si>
-  <si>
-    <t>Text Dateien</t>
-  </si>
-  <si>
-    <t>Ficheros en texto plano</t>
-  </si>
-  <si>
-    <t>Fichiers texte bruts</t>
-  </si>
-  <si>
-    <t>File di testo semplice</t>
-  </si>
-  <si>
-    <t>Zwykłe pliki tekstowe</t>
-  </si>
-  <si>
-    <t>Fișiere cu text simplu</t>
-  </si>
-  <si>
-    <t>Текстовые файлы</t>
-  </si>
-  <si>
-    <t>纯文本文件</t>
-  </si>
-  <si>
-    <t>純文字檔案</t>
+    <t>Markdown/Plain Text Files</t>
+  </si>
+  <si>
+    <t>Markdown/Textové soubory</t>
+  </si>
+  <si>
+    <t>Markdown/Text Dateien</t>
+  </si>
+  <si>
+    <t>Ficheros en Markdown/texto plano</t>
+  </si>
+  <si>
+    <t>Markdown/Fichiers texte bruts</t>
+  </si>
+  <si>
+    <t>File di Markdown/testo semplice</t>
+  </si>
+  <si>
+    <t>Markdown/Zwykłe pliki tekstowe</t>
+  </si>
+  <si>
+    <t>Fișiere cu Markdown/text simplu</t>
+  </si>
+  <si>
+    <t>Markdown/Текстовые файлы</t>
+  </si>
+  <si>
+    <t>Markdown/纯文本文件</t>
+  </si>
+  <si>
+    <t>Markdown/純文字檔案</t>
   </si>
   <si>
     <t>plain_text_files_help</t>
   </si>
   <si>
-    <t>In order to import your Notes from plain text files (single file or folder), click Import. Every file is imported as a separate note, the file’s name becomes the note’s title. If the text contents start with list syntax (e.g. Markdown ’- [x]’, NotallyX syntax ’[✓]’, or ’*’, ’-’) it will be converted to a List note.</t>
+    <t>In order to import your Notes from markdown/plain text files (single file or folder), click Import. Every file is imported as a separate note, the file’s name becomes the note’s title. If the text contents start with list syntax (e.g. Markdown ’- [x]’, NotallyX syntax ’[✓]’, or ’*’, ’-’) it will be converted to a List note.</t>
   </si>
   <si>
     <t>Chcete-li importovat poznámky z textových souborů (jednotlivých souborů nebo složek), klikněte na tlačítko Importovat. Každý soubor se importuje jako samostatná poznámka, název souboru se stane názvem poznámky. Pokud textový obsah začíná syntaxí seznamu (např. syntaxí Markdown '- [x]', NotallyX '[✓]' nebo '*', '-'), bude převeden na poznámku Seznam.</t>

</xml_diff>